<commit_message>
21 Apr 2020 Updates
The two videos today were long and involved several files.

World Covid Status 21 Apr 2020 and a Long Discussion on Solving Global Problems
https://youtu.be/effG-S3SGFU
Using Logistic Projection Cumulative Normal Projection for a Few Countries and The World
https://youtu.be/BxfrcvxEric
</commit_message>
<xml_diff>
--- a/Analyses/World Deaths from Respiratory Disease.xlsx
+++ b/Analyses/World Deaths from Respiratory Disease.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Server\$MyViewer\$Bang1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\World-Covid-Status-Notes\Analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="182">
   <si>
     <t>Country-years:
    South Africa (2015)
@@ -590,6 +590,12 @@
   </si>
   <si>
     <t>Cumulative Percent</t>
+  </si>
+  <si>
+    <t>Log Rate Older</t>
+  </si>
+  <si>
+    <t>Log Rate Younger</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1344,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'WHO Deaths Respiratory'!$D$2</c:f>
+              <c:f>'WHO Deaths Respiratory'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1444,7 +1450,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'WHO Deaths Respiratory'!$D$3:$D$27</c:f>
+              <c:f>'WHO Deaths Respiratory'!$F$3:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1537,11 +1543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="339820744"/>
-        <c:axId val="339822704"/>
+        <c:axId val="508102824"/>
+        <c:axId val="508103216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="339820744"/>
+        <c:axId val="508102824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339822704"/>
+        <c:crossAx val="508103216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1592,7 +1598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="339822704"/>
+        <c:axId val="508103216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,7 +1649,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339820744"/>
+        <c:crossAx val="508102824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1739,6 +1745,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2445,11 +2452,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="341349272"/>
-        <c:axId val="341349664"/>
+        <c:axId val="413031192"/>
+        <c:axId val="413031584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="341349272"/>
+        <c:axId val="413031192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,12 +2512,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341349664"/>
+        <c:crossAx val="413031584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="341349664"/>
+        <c:axId val="413031584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,7 +2574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341349272"/>
+        <c:crossAx val="413031192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2581,6 +2588,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2662,6 +2670,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3368,11 +3377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="341350448"/>
-        <c:axId val="335931096"/>
+        <c:axId val="346526992"/>
+        <c:axId val="346527384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="341350448"/>
+        <c:axId val="346526992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3428,12 +3437,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335931096"/>
+        <c:crossAx val="346527384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335931096"/>
+        <c:axId val="346527384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3490,7 +3499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341350448"/>
+        <c:crossAx val="346526992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3504,6 +3513,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3626,6 +3636,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4332,11 +4343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335931880"/>
-        <c:axId val="335932272"/>
+        <c:axId val="346528168"/>
+        <c:axId val="420219336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335931880"/>
+        <c:axId val="346528168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4392,12 +4403,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335932272"/>
+        <c:crossAx val="420219336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335932272"/>
+        <c:axId val="420219336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4454,7 +4465,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335931880"/>
+        <c:crossAx val="346528168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4559,7 +4570,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'WHO Deaths Respiratory'!$D$2</c:f>
+              <c:f>'WHO Deaths Respiratory'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4675,7 +4686,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'WHO Deaths Respiratory'!$D$3:$D$26</c:f>
+              <c:f>'WHO Deaths Respiratory'!$F$3:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
@@ -4764,11 +4775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="264856728"/>
-        <c:axId val="264855944"/>
+        <c:axId val="508209704"/>
+        <c:axId val="508210096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="264856728"/>
+        <c:axId val="508209704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4825,12 +4836,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264855944"/>
+        <c:crossAx val="508210096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="264855944"/>
+        <c:axId val="508210096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4887,7 +4898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264856728"/>
+        <c:crossAx val="508209704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4951,6 +4962,40 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Respiratory Death Rate</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Per Millions Shape</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -5486,11 +5531,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335761904"/>
-        <c:axId val="335762296"/>
+        <c:axId val="508104000"/>
+        <c:axId val="344338248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335761904"/>
+        <c:axId val="508104000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5547,14 +5592,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335762296"/>
+        <c:crossAx val="344338248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335762296"/>
+        <c:axId val="344338248"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5610,7 +5654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335761904"/>
+        <c:crossAx val="508104000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5674,6 +5718,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Log10</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Respiratory Death Rates Per Millions</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Sample Young and Old </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -5715,11 +5798,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'WHO Deaths Respiratory'!$C$2</c:f>
+              <c:f>'WHO Deaths Respiratory'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rate per Million</c:v>
+                  <c:v>Log Rate Older</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5734,261 +5817,20 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'WHO Deaths Respiratory'!$B$3:$B$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>97</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'WHO Deaths Respiratory'!$C$3:$C$26</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>39.683206610034667</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.2464836696579322</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.9426399100305782</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1944623960581247</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8163760909747904</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2431531683721053</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2771583433326981</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.9242204105946596</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.862462790871291</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.5603426685873893</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.3365900312389103</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.0250191095189312</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.513873006257187</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20.141179803224283</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>36.27858094387944</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>67.178182048711918</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>120.22042853889185</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>208.83483461316536</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>399.4173566024989</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>806.71813294125411</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1524.3105731254943</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3182.1964069779947</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5041.5745152895706</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8718.1826274112991</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'WHO Deaths Respiratory'!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Rate per Million</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="C00000"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -6023,20 +5865,6 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'WHO Deaths Respiratory'!$B$3:$B$26</c:f>
@@ -6120,81 +5948,199 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'WHO Deaths Respiratory'!$C$3:$C$26</c:f>
+              <c:f>'WHO Deaths Respiratory'!$D$3:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="6">
+                  <c:v>0.10624474485348702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28425481698582938</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45673984999447564</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65899747720068047</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8018556097715589</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95544813015108476</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1307798334182531</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3040849064868607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5596502910590682</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8272282469469134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0799782717256301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.3198029426944804</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6014269331258428</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.9067218188715884</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.1830734620514849</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.5027269810410346</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.7025661905155229</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9404259623240412</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'WHO Deaths Respiratory'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log Rate Younger</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'WHO Deaths Respiratory'!$B$3:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'WHO Deaths Respiratory'!$E$3:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>39.683206610034667</c:v>
+                  <c:v>1.5986067581589798</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2464836696579322</c:v>
+                  <c:v>0.96597660698758925</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9426399100305782</c:v>
+                  <c:v>0.59578711381479355</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1944623960581247</c:v>
+                  <c:v>0.34132814324689426</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8163760909747904</c:v>
+                  <c:v>0.25920577663233385</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2431531683721053</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2771583433326981</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.9242204105946596</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.862462790871291</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.5603426685873893</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.3365900312389103</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.0250191095189312</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.513873006257187</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20.141179803224283</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>36.27858094387944</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>67.178182048711918</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>120.22042853889185</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>208.83483461316536</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>399.4173566024989</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>806.71813294125411</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1524.3105731254943</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3182.1964069779947</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5041.5745152895706</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8718.1826274112991</c:v>
+                  <c:v>9.4524641176381444E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6209,11 +6155,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335762688"/>
-        <c:axId val="335763080"/>
+        <c:axId val="504083536"/>
+        <c:axId val="504085496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335762688"/>
+        <c:axId val="504083536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6270,12 +6216,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335763080"/>
+        <c:crossAx val="504085496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335763080"/>
+        <c:axId val="504085496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6332,7 +6278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335762688"/>
+        <c:crossAx val="504083536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6344,6 +6290,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6581,11 +6559,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335761120"/>
-        <c:axId val="335763472"/>
+        <c:axId val="508210880"/>
+        <c:axId val="344338640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335761120"/>
+        <c:axId val="508210880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6642,12 +6620,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335763472"/>
+        <c:crossAx val="344338640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335763472"/>
+        <c:axId val="344338640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6704,7 +6682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335761120"/>
+        <c:crossAx val="508210880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7031,11 +7009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="259497248"/>
-        <c:axId val="259494896"/>
+        <c:axId val="344339424"/>
+        <c:axId val="344339816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="259497248"/>
+        <c:axId val="344339424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7092,12 +7070,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259494896"/>
+        <c:crossAx val="344339816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="259494896"/>
+        <c:axId val="344339816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7154,7 +7132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259497248"/>
+        <c:crossAx val="344339424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7522,11 +7500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335764256"/>
-        <c:axId val="339823880"/>
+        <c:axId val="424678520"/>
+        <c:axId val="512452816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335764256"/>
+        <c:axId val="424678520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7583,12 +7561,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339823880"/>
+        <c:crossAx val="512452816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339823880"/>
+        <c:axId val="512452816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7645,7 +7623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335764256"/>
+        <c:crossAx val="424678520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7928,11 +7906,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="341346920"/>
-        <c:axId val="341347312"/>
+        <c:axId val="512453600"/>
+        <c:axId val="512453992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="341346920"/>
+        <c:axId val="512453600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7989,12 +7967,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341347312"/>
+        <c:crossAx val="512453992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="341347312"/>
+        <c:axId val="512453992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8051,7 +8029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341346920"/>
+        <c:crossAx val="512453600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8165,6 +8143,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8873,11 +8852,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="341348096"/>
-        <c:axId val="341348488"/>
+        <c:axId val="413030016"/>
+        <c:axId val="413030408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341348096"/>
+        <c:axId val="413030016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8920,7 +8899,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341348488"/>
+        <c:crossAx val="413030408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8928,7 +8907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341348488"/>
+        <c:axId val="413030408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8979,7 +8958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341348096"/>
+        <c:crossAx val="413030016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15691,13 +15670,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>186690</xdr:rowOff>
@@ -15721,13 +15700,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
@@ -15751,21 +15730,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -15781,23 +15762,21 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>80010</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>384810</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -16337,7 +16316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="G26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -21585,21 +21564,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O103"/>
+  <dimension ref="A2:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -21610,19 +21590,25 @@
         <v>176</v>
       </c>
       <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>175</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -21630,24 +21616,29 @@
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C26" si="0">D3/E3</f>
+        <f t="shared" ref="C3:C26" si="0">F3/G3</f>
         <v>39.683206610034667</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
+        <f>LOG10(C3)</f>
+        <v>1.5986067581589798</v>
+      </c>
+      <c r="F3" s="7">
         <v>5400</v>
       </c>
-      <c r="E3" s="14">
-        <f>+O3</f>
+      <c r="G3" s="14">
+        <f>+Q3</f>
         <v>136.07771299999999</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="12">
+      <c r="Q3" s="12">
         <v>136.07771299999999</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -21658,21 +21649,26 @@
         <f t="shared" si="0"/>
         <v>9.2464836696579322</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
+        <f t="shared" ref="E4:E8" si="1">LOG10(C4)</f>
+        <v>0.96597660698758925</v>
+      </c>
+      <c r="F4" s="7">
         <v>1257</v>
       </c>
-      <c r="E4" s="14">
-        <f>+O4</f>
+      <c r="G4" s="14">
+        <f>+Q4</f>
         <v>135.94356999999999</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="12">
+      <c r="Q4" s="12">
         <v>135.94356999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -21683,21 +21679,26 @@
         <f t="shared" si="0"/>
         <v>3.9426399100305782</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.59578711381479355</v>
+      </c>
+      <c r="F5" s="7">
         <v>535</v>
       </c>
-      <c r="E5" s="14">
-        <f>+O5</f>
+      <c r="G5" s="14">
+        <f>+Q5</f>
         <v>135.69588200000001</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O5" s="12">
+      <c r="Q5" s="12">
         <v>135.69588200000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -21708,21 +21709,26 @@
         <f t="shared" si="0"/>
         <v>2.1944623960581247</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.34132814324689426</v>
+      </c>
+      <c r="F6" s="7">
         <v>297</v>
       </c>
-      <c r="E6" s="14">
-        <f>+O6</f>
+      <c r="G6" s="14">
+        <f>+Q6</f>
         <v>135.340665</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="12">
+      <c r="Q6" s="12">
         <v>135.340665</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -21733,21 +21739,26 @@
         <f t="shared" si="0"/>
         <v>1.8163760909747904</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.25920577663233385</v>
+      </c>
+      <c r="F7" s="7">
         <v>245</v>
       </c>
-      <c r="E7" s="14">
-        <f>+O7</f>
+      <c r="G7" s="14">
+        <f>+Q7</f>
         <v>134.88396</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="12">
+      <c r="Q7" s="12">
         <v>134.88396</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -21758,21 +21769,26 @@
         <f t="shared" si="0"/>
         <v>1.2431531683721053</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>9.4524641176381444E-2</v>
+      </c>
+      <c r="F8" s="7">
         <v>826</v>
       </c>
-      <c r="E8" s="14">
-        <f>SUM(O8:O12)</f>
+      <c r="G8" s="14">
+        <f>SUM(Q8:Q12)</f>
         <v>664.43944399999998</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="O8" s="12">
+      <c r="Q8" s="12">
         <v>134.33180400000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -21783,21 +21799,26 @@
         <f t="shared" si="0"/>
         <v>1.2771583433326981</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
+        <f>LOG10(C9)</f>
+        <v>0.10624474485348702</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7">
         <v>819</v>
       </c>
-      <c r="E9" s="14">
-        <f>SUM(O13:O17)</f>
+      <c r="G9" s="14">
+        <f>SUM(Q13:Q17)</f>
         <v>641.26739200000009</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="12">
+      <c r="Q9" s="12">
         <v>133.69022099999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -21809,21 +21830,26 @@
         <f t="shared" si="0"/>
         <v>1.9242204105946596</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
+        <f t="shared" ref="D10:D26" si="2">LOG10(C10)</f>
+        <v>0.28425481698582938</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7">
         <v>1178</v>
       </c>
-      <c r="E10" s="14">
-        <f>SUM(O18:O22)</f>
+      <c r="G10" s="14">
+        <f>SUM(Q18:Q22)</f>
         <v>612.19597999999996</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="P10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="O10" s="12">
+      <c r="Q10" s="12">
         <v>132.96523499999998</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -21835,1029 +21861,1109 @@
         <f t="shared" si="0"/>
         <v>2.862462790871291</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
+        <f t="shared" si="2"/>
+        <v>0.45673984999447564</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7">
         <v>1710</v>
       </c>
-      <c r="E11" s="14">
-        <f>SUM(O23:O27)</f>
+      <c r="G11" s="14">
+        <f>SUM(Q23:Q27)</f>
         <v>597.38767799999994</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="P11" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="O11" s="12">
+      <c r="Q11" s="12">
         <v>132.162924</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:B26" si="1">+B11+5</f>
+        <f t="shared" ref="B12:B26" si="3">+B11+5</f>
         <v>27</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
         <v>4.5603426685873893</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
+        <f t="shared" si="2"/>
+        <v>0.65899747720068047</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7">
         <v>2712</v>
       </c>
-      <c r="E12" s="14">
-        <f>SUM(O28:O32)</f>
+      <c r="G12" s="14">
+        <f>SUM(Q28:Q32)</f>
         <v>594.69215299999996</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="P12" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="12">
+      <c r="Q12" s="12">
         <v>131.28926000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
         <v>6.3365900312389103</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
+        <f t="shared" si="2"/>
+        <v>0.8018556097715589</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7">
         <v>3837</v>
       </c>
-      <c r="E13" s="14">
-        <f>SUM(O33:O37)</f>
+      <c r="G13" s="14">
+        <f>SUM(Q33:Q37)</f>
         <v>605.53073199999994</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="P13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="O13" s="12">
+      <c r="Q13" s="12">
         <v>130.37654000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
         <v>9.0250191095189312</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.95544813015108476</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7">
         <v>4917</v>
       </c>
-      <c r="E14" s="14">
-        <f>SUM(O38:O42)</f>
+      <c r="G14" s="14">
+        <f>SUM(Q38:Q42)</f>
         <v>544.81879099999992</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="P14" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="12">
+      <c r="Q14" s="12">
         <v>129.45701199999999</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
         <v>13.513873006257187</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1307798334182531</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7">
         <v>6673</v>
       </c>
-      <c r="E15" s="14">
-        <f>SUM(O43:O47)</f>
+      <c r="G15" s="14">
+        <f>SUM(Q43:Q47)</f>
         <v>493.78886399999993</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="P15" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="O15" s="12">
+      <c r="Q15" s="12">
         <v>128.40558300000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
         <v>20.141179803224283</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3040849064868607</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7">
         <v>9655</v>
       </c>
-      <c r="E16" s="14">
-        <f>SUM(O48:O52)</f>
+      <c r="G16" s="14">
+        <f>SUM(Q48:Q52)</f>
         <v>479.36615899999998</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="P16" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="O16" s="12">
+      <c r="Q16" s="12">
         <v>127.175817</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
         <v>36.27858094387944</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5596502910590682</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7">
         <v>16172</v>
       </c>
-      <c r="E17" s="14">
-        <f>SUM(O53:O57)</f>
+      <c r="G17" s="14">
+        <f>SUM(Q53:Q57)</f>
         <v>445.772673</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="P17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="O17" s="12">
+      <c r="Q17" s="12">
         <v>125.85244</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
         <v>67.178182048711918</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8272282469469134</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7">
         <v>26055</v>
       </c>
-      <c r="E18" s="14">
-        <f>SUM(O58:O62)</f>
+      <c r="G18" s="14">
+        <f>SUM(Q58:Q62)</f>
         <v>387.8491380000001</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="P18" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="O18" s="12">
+      <c r="Q18" s="12">
         <v>124.56313</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
         <v>120.22042853889185</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
+        <f t="shared" si="2"/>
+        <v>2.0799782717256301</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7">
         <v>38728</v>
       </c>
-      <c r="E19" s="14">
-        <f>SUM(O63:O67)</f>
+      <c r="G19" s="14">
+        <f>SUM(Q63:Q67)</f>
         <v>322.14159000000001</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="P19" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O19" s="12">
+      <c r="Q19" s="12">
         <v>123.27823600000001</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
         <v>208.83483461316536</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3198029426944804</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7">
         <v>56311</v>
       </c>
-      <c r="E20" s="14">
-        <f>SUM(O68:O72)</f>
+      <c r="G20" s="14">
+        <f>SUM(Q68:Q72)</f>
         <v>269.64371200000005</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="P20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O20" s="12">
+      <c r="Q20" s="12">
         <v>122.18228500000001</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
         <v>399.4173566024989</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
+        <f t="shared" si="2"/>
+        <v>2.6014269331258428</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7">
         <v>75361</v>
       </c>
-      <c r="E21" s="14">
-        <f>SUM(O73:O77)</f>
+      <c r="G21" s="14">
+        <f>SUM(Q73:Q77)</f>
         <v>188.67732899999999</v>
       </c>
-      <c r="N21" s="11" t="s">
+      <c r="P21" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="O21" s="12">
+      <c r="Q21" s="12">
         <v>121.37895399999999</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
         <v>806.71813294125411</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
+        <f t="shared" si="2"/>
+        <v>2.9067218188715884</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7">
         <v>99857</v>
       </c>
-      <c r="E22" s="14">
-        <f>SUM(O78:O82)</f>
+      <c r="G22" s="14">
+        <f>SUM(Q78:Q82)</f>
         <v>123.78177199999999</v>
       </c>
-      <c r="N22" s="11" t="s">
+      <c r="P22" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="O22" s="12">
+      <c r="Q22" s="12">
         <v>120.793375</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
         <v>1524.3105731254943</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1830734620514849</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7">
         <v>124887</v>
       </c>
-      <c r="E23" s="14">
-        <f>SUM(O83:O87)</f>
+      <c r="G23" s="14">
+        <f>SUM(Q83:Q87)</f>
         <v>81.930153999999987</v>
       </c>
-      <c r="N23" s="11" t="s">
+      <c r="P23" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="O23" s="12">
+      <c r="Q23" s="12">
         <v>120.249348</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
         <v>3182.1964069779947</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5027269810410346</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7">
         <v>134245</v>
       </c>
-      <c r="E24" s="14">
-        <f>SUM(O88:O92)</f>
+      <c r="G24" s="14">
+        <f>SUM(Q88:Q92)</f>
         <v>42.186271000000005</v>
       </c>
-      <c r="N24" s="11" t="s">
+      <c r="P24" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="O24" s="12">
+      <c r="Q24" s="12">
         <v>119.784802</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
         <v>5041.5745152895706</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
+        <f t="shared" si="2"/>
+        <v>3.7025661905155229</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7">
         <v>90328</v>
       </c>
-      <c r="E25" s="14">
-        <f>SUM(O93:O98)</f>
+      <c r="G25" s="14">
+        <f>SUM(Q93:Q98)</f>
         <v>17.916625</v>
       </c>
-      <c r="N25" s="11" t="s">
+      <c r="P25" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="O25" s="12">
+      <c r="Q25" s="12">
         <v>119.40349999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
         <v>8718.1826274112991</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
+        <f t="shared" si="2"/>
+        <v>3.9404259623240412</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7">
         <v>41037</v>
       </c>
-      <c r="E26" s="14">
-        <f>SUM(O98:O103)</f>
+      <c r="G26" s="14">
+        <f>SUM(Q98:Q103)</f>
         <v>4.7070590000000001</v>
       </c>
-      <c r="N26" s="11" t="s">
+      <c r="P26" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="O26" s="12">
+      <c r="Q26" s="12">
         <v>119.09049899999999</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>110</v>
       </c>
-      <c r="N27" s="11" t="s">
+      <c r="P27" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="O27" s="12">
+      <c r="Q27" s="12">
         <v>118.85952899999999</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N28" s="11" t="s">
+    <row r="28" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="O28" s="12">
+      <c r="Q28" s="12">
         <v>118.60303999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N29" s="11" t="s">
+    <row r="29" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P29" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="O29" s="12">
+      <c r="Q29" s="12">
         <v>118.179163</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N30" s="11" t="s">
+    <row r="30" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P30" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="O30" s="12">
+      <c r="Q30" s="12">
         <v>118.276518</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N31" s="11" t="s">
+    <row r="31" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P31" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="O31" s="12">
+      <c r="Q31" s="12">
         <v>119.17419500000001</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N32" s="11" t="s">
+    <row r="32" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P32" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="O32" s="12">
+      <c r="Q32" s="12">
         <v>120.45923699999999</v>
       </c>
     </row>
-    <row r="33" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N33" s="11" t="s">
+    <row r="33" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P33" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="O33" s="12">
+      <c r="Q33" s="12">
         <v>121.569568</v>
       </c>
     </row>
-    <row r="34" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N34" s="11" t="s">
+    <row r="34" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P34" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O34" s="12">
+      <c r="Q34" s="12">
         <v>122.773552</v>
       </c>
     </row>
-    <row r="35" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N35" s="11" t="s">
+    <row r="35" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P35" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="O35" s="12">
+      <c r="Q35" s="12">
         <v>122.742987</v>
       </c>
     </row>
-    <row r="36" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N36" s="11" t="s">
+    <row r="36" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P36" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="O36" s="12">
+      <c r="Q36" s="12">
         <v>120.809448</v>
       </c>
     </row>
-    <row r="37" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N37" s="11" t="s">
+    <row r="37" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P37" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="O37" s="12">
+      <c r="Q37" s="12">
         <v>117.635177</v>
       </c>
     </row>
-    <row r="38" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N38" s="11" t="s">
+    <row r="38" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P38" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="O38" s="12">
+      <c r="Q38" s="12">
         <v>114.59375</v>
       </c>
     </row>
-    <row r="39" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N39" s="11" t="s">
+    <row r="39" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P39" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="O39" s="12">
+      <c r="Q39" s="12">
         <v>111.462159</v>
       </c>
     </row>
-    <row r="40" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N40" s="11" t="s">
+    <row r="40" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P40" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="O40" s="12">
+      <c r="Q40" s="12">
         <v>108.538738</v>
       </c>
     </row>
-    <row r="41" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N41" s="11" t="s">
+    <row r="41" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P41" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="O41" s="12">
+      <c r="Q41" s="12">
         <v>106.12721999999999</v>
       </c>
     </row>
-    <row r="42" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N42" s="11" t="s">
+    <row r="42" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P42" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="O42" s="12">
+      <c r="Q42" s="12">
         <v>104.096924</v>
       </c>
     </row>
-    <row r="43" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N43" s="11" t="s">
+    <row r="43" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P43" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="O43" s="12">
+      <c r="Q43" s="12">
         <v>101.924132</v>
       </c>
     </row>
-    <row r="44" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N44" s="11" t="s">
+    <row r="44" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P44" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="O44" s="12">
+      <c r="Q44" s="12">
         <v>99.606488999999996</v>
       </c>
     </row>
-    <row r="45" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N45" s="11" t="s">
+    <row r="45" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P45" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="O45" s="12">
+      <c r="Q45" s="12">
         <v>97.93562399999999</v>
       </c>
     </row>
-    <row r="46" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N46" s="11" t="s">
+    <row r="46" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P46" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="O46" s="12">
+      <c r="Q46" s="12">
         <v>97.219210000000004</v>
       </c>
     </row>
-    <row r="47" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N47" s="11" t="s">
+    <row r="47" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P47" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="O47" s="12">
+      <c r="Q47" s="12">
         <v>97.103408999999999</v>
       </c>
     </row>
-    <row r="48" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N48" s="11" t="s">
+    <row r="48" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P48" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="O48" s="12">
+      <c r="Q48" s="12">
         <v>96.918301999999997</v>
       </c>
     </row>
-    <row r="49" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N49" s="11" t="s">
+    <row r="49" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P49" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="O49" s="12">
+      <c r="Q49" s="12">
         <v>96.787975000000003</v>
       </c>
     </row>
-    <row r="50" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N50" s="11" t="s">
+    <row r="50" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P50" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="O50" s="12">
+      <c r="Q50" s="12">
         <v>96.35055899999999</v>
       </c>
     </row>
-    <row r="51" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N51" s="11" t="s">
+    <row r="51" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P51" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="O51" s="12">
+      <c r="Q51" s="12">
         <v>95.35482300000001</v>
       </c>
     </row>
-    <row r="52" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N52" s="11" t="s">
+    <row r="52" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P52" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="O52" s="12">
+      <c r="Q52" s="12">
         <v>93.954499999999996</v>
       </c>
     </row>
-    <row r="53" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N53" s="11" t="s">
+    <row r="53" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P53" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="O53" s="12">
+      <c r="Q53" s="12">
         <v>92.581013999999996</v>
       </c>
     </row>
-    <row r="54" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N54" s="11" t="s">
+    <row r="54" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P54" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="O54" s="12">
+      <c r="Q54" s="12">
         <v>91.179835000000011</v>
       </c>
     </row>
-    <row r="55" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N55" s="11" t="s">
+    <row r="55" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P55" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="O55" s="12">
+      <c r="Q55" s="12">
         <v>89.488096000000112</v>
       </c>
     </row>
-    <row r="56" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N56" s="11" t="s">
+    <row r="56" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P56" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="O56" s="12">
+      <c r="Q56" s="12">
         <v>87.428042999999903</v>
       </c>
     </row>
-    <row r="57" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N57" s="11" t="s">
+    <row r="57" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P57" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="O57" s="12">
+      <c r="Q57" s="12">
         <v>85.095685000000003</v>
       </c>
     </row>
-    <row r="58" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N58" s="11" t="s">
+    <row r="58" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P58" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="O58" s="12">
+      <c r="Q58" s="12">
         <v>82.698174000000094</v>
       </c>
     </row>
-    <row r="59" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N59" s="11" t="s">
+    <row r="59" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P59" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="O59" s="12">
+      <c r="Q59" s="12">
         <v>80.234426999999997</v>
       </c>
     </row>
-    <row r="60" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N60" s="11" t="s">
+    <row r="60" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P60" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="O60" s="12">
+      <c r="Q60" s="12">
         <v>77.660567</v>
       </c>
     </row>
-    <row r="61" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N61" s="11" t="s">
+    <row r="61" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P61" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="O61" s="12">
+      <c r="Q61" s="12">
         <v>74.988858999999991</v>
       </c>
     </row>
-    <row r="62" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N62" s="11" t="s">
+    <row r="62" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P62" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="O62" s="12">
+      <c r="Q62" s="12">
         <v>72.267111</v>
       </c>
     </row>
-    <row r="63" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N63" s="11" t="s">
+    <row r="63" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P63" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="O63" s="12">
+      <c r="Q63" s="12">
         <v>69.464247</v>
       </c>
     </row>
-    <row r="64" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N64" s="11" t="s">
+    <row r="64" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P64" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="O64" s="12">
+      <c r="Q64" s="12">
         <v>66.506443000000004</v>
       </c>
     </row>
-    <row r="65" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N65" s="11" t="s">
+    <row r="65" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P65" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="O65" s="12">
+      <c r="Q65" s="12">
         <v>63.921533000000004</v>
       </c>
     </row>
-    <row r="66" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N66" s="11" t="s">
+    <row r="66" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P66" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="O66" s="12">
+      <c r="Q66" s="12">
         <v>61.943697</v>
       </c>
     </row>
-    <row r="67" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N67" s="11" t="s">
+    <row r="67" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P67" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="O67" s="12">
+      <c r="Q67" s="12">
         <v>60.305669999999999</v>
       </c>
     </row>
-    <row r="68" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N68" s="11" t="s">
+    <row r="68" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P68" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="O68" s="12">
+      <c r="Q68" s="12">
         <v>58.577354</v>
       </c>
     </row>
-    <row r="69" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N69" s="11" t="s">
+    <row r="69" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P69" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="O69" s="13">
+      <c r="Q69" s="13">
         <v>56.930253</v>
       </c>
     </row>
-    <row r="70" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N70" s="11" t="s">
+    <row r="70" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P70" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="O70" s="13">
+      <c r="Q70" s="13">
         <v>54.708286999999999</v>
       </c>
     </row>
-    <row r="71" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N71" s="11" t="s">
+    <row r="71" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P71" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="O71" s="13">
+      <c r="Q71" s="13">
         <v>51.568814000000103</v>
       </c>
     </row>
-    <row r="72" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N72" s="11" t="s">
+    <row r="72" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P72" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="O72" s="13">
+      <c r="Q72" s="13">
         <v>47.859003999999999</v>
       </c>
     </row>
-    <row r="73" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N73" s="11" t="s">
+    <row r="73" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P73" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="O73" s="13">
+      <c r="Q73" s="13">
         <v>44.279766000000002</v>
       </c>
     </row>
-    <row r="74" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N74" s="11" t="s">
+    <row r="74" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P74" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="O74" s="13">
+      <c r="Q74" s="13">
         <v>40.704317000000003</v>
       </c>
     </row>
-    <row r="75" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N75" s="11" t="s">
+    <row r="75" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P75" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="O75" s="13">
+      <c r="Q75" s="13">
         <v>37.366478000000001</v>
       </c>
     </row>
-    <row r="76" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N76" s="11" t="s">
+    <row r="76" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P76" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="O76" s="13">
+      <c r="Q76" s="13">
         <v>34.457741999999996</v>
       </c>
     </row>
-    <row r="77" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N77" s="11" t="s">
+    <row r="77" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P77" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="O77" s="13">
+      <c r="Q77" s="13">
         <v>31.869026000000002</v>
       </c>
     </row>
-    <row r="78" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N78" s="11" t="s">
+    <row r="78" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P78" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="O78" s="13">
+      <c r="Q78" s="13">
         <v>29.266348000000001</v>
       </c>
     </row>
-    <row r="79" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N79" s="11" t="s">
+    <row r="79" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P79" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="O79" s="12">
+      <c r="Q79" s="12">
         <v>26.676295</v>
       </c>
     </row>
-    <row r="80" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N80" s="11" t="s">
+    <row r="80" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P80" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="O80" s="12">
+      <c r="Q80" s="12">
         <v>24.393371999999999</v>
       </c>
     </row>
-    <row r="81" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N81" s="11" t="s">
+    <row r="81" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P81" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="O81" s="12">
+      <c r="Q81" s="12">
         <v>22.518103</v>
       </c>
     </row>
-    <row r="82" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N82" s="11" t="s">
+    <row r="82" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P82" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="O82" s="12">
+      <c r="Q82" s="12">
         <v>20.927653999999997</v>
       </c>
     </row>
-    <row r="83" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N83" s="11" t="s">
+    <row r="83" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P83" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="O83" s="12">
+      <c r="Q83" s="12">
         <v>19.418133000000001</v>
       </c>
     </row>
-    <row r="84" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N84" s="11" t="s">
+    <row r="84" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P84" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="O84" s="12">
+      <c r="Q84" s="12">
         <v>18.053656</v>
       </c>
     </row>
-    <row r="85" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N85" s="11" t="s">
+    <row r="85" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P85" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="O85" s="12">
+      <c r="Q85" s="12">
         <v>16.580794999999998</v>
       </c>
     </row>
-    <row r="86" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N86" s="11" t="s">
+    <row r="86" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P86" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="O86" s="12">
+      <c r="Q86" s="12">
         <v>14.860267</v>
       </c>
     </row>
-    <row r="87" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N87" s="11" t="s">
+    <row r="87" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P87" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="O87" s="12">
+      <c r="Q87" s="12">
         <v>13.017303</v>
       </c>
     </row>
-    <row r="88" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N88" s="11" t="s">
+    <row r="88" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P88" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="O88" s="12">
+      <c r="Q88" s="12">
         <v>11.314382</v>
       </c>
     </row>
-    <row r="89" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N89" s="11" t="s">
+    <row r="89" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P89" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="O89" s="12">
+      <c r="Q89" s="12">
         <v>9.696530000000001</v>
       </c>
     </row>
-    <row r="90" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N90" s="11" t="s">
+    <row r="90" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P90" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="O90" s="12">
+      <c r="Q90" s="12">
         <v>8.2375450000000008</v>
       </c>
     </row>
-    <row r="91" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N91" s="11" t="s">
+    <row r="91" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P91" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="O91" s="12">
+      <c r="Q91" s="12">
         <v>6.9997259999999999</v>
       </c>
     </row>
-    <row r="92" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N92" s="11" t="s">
+    <row r="92" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P92" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="O92" s="12">
+      <c r="Q92" s="12">
         <v>5.9380879999999996</v>
       </c>
     </row>
-    <row r="93" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N93" s="11" t="s">
+    <row r="93" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P93" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="O93" s="12">
+      <c r="Q93" s="12">
         <v>4.8287420000000001</v>
       </c>
     </row>
-    <row r="94" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N94" s="11" t="s">
+    <row r="94" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P94" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="O94" s="12">
+      <c r="Q94" s="12">
         <v>3.993554</v>
       </c>
     </row>
-    <row r="95" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N95" s="11" t="s">
+    <row r="95" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P95" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="O95" s="12">
+      <c r="Q95" s="12">
         <v>3.4087589999999999</v>
       </c>
     </row>
-    <row r="96" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N96" s="11" t="s">
+    <row r="96" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P96" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="O96" s="12">
+      <c r="Q96" s="12">
         <v>2.670423</v>
       </c>
     </row>
-    <row r="97" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N97" s="11" t="s">
+    <row r="97" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P97" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="O97" s="12">
+      <c r="Q97" s="12">
         <v>1.77857</v>
       </c>
     </row>
-    <row r="98" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N98" s="11" t="s">
+    <row r="98" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P98" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="O98" s="12">
+      <c r="Q98" s="12">
         <v>1.236577</v>
       </c>
     </row>
-    <row r="99" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N99" s="11" t="s">
+    <row r="99" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P99" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="O99" s="12">
+      <c r="Q99" s="12">
         <v>1.0662339999999999</v>
       </c>
     </row>
-    <row r="100" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N100" s="11" t="s">
+    <row r="100" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P100" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="O100" s="12">
+      <c r="Q100" s="12">
         <v>0.86130700000000004</v>
       </c>
     </row>
-    <row r="101" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N101" s="11" t="s">
+    <row r="101" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P101" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="O101" s="12">
+      <c r="Q101" s="12">
         <v>0.62180499999999994</v>
       </c>
     </row>
-    <row r="102" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N102" s="11" t="s">
+    <row r="102" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P102" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="O102" s="12">
+      <c r="Q102" s="12">
         <v>0.34771300000000005</v>
       </c>
     </row>
-    <row r="103" spans="14:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N103" s="11" t="s">
+    <row r="103" spans="16:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P103" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="O103" s="12">
+      <c r="Q103" s="12">
         <v>0.57342300000000002</v>
       </c>
     </row>
@@ -22871,7 +22977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:T28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
@@ -23870,7 +23976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>

</xml_diff>